<commit_message>
Function has been enhaced for Exporting All and filtered data.
</commit_message>
<xml_diff>
--- a/backend/exports/all_requirements.xlsx
+++ b/backend/exports/all_requirements.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M281"/>
+  <dimension ref="A1:M341"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15760,6 +15760,3306 @@
         <v>1</v>
       </c>
     </row>
+    <row r="282">
+      <c r="A282" t="inlineStr">
+        <is>
+          <t>Afsar Khan</t>
+        </is>
+      </c>
+      <c r="B282" t="inlineStr">
+        <is>
+          <t>REDX_VMS Portal</t>
+        </is>
+      </c>
+      <c r="C282" t="inlineStr">
+        <is>
+          <t>Mumbai Maharashtra India</t>
+        </is>
+      </c>
+      <c r="D282" t="inlineStr">
+        <is>
+          <t>Mr.Nitin</t>
+        </is>
+      </c>
+      <c r="E282" t="n">
+        <v>4.17</v>
+      </c>
+      <c r="F282" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="G282" t="inlineStr">
+        <is>
+          <t>Honeywell</t>
+        </is>
+      </c>
+      <c r="H282" t="inlineStr">
+        <is>
+          <t>5MP (2560x1920)</t>
+        </is>
+      </c>
+      <c r="I282" t="n">
+        <v>25</v>
+      </c>
+      <c r="J282" t="inlineStr">
+        <is>
+          <t>H265</t>
+        </is>
+      </c>
+      <c r="K282" t="n">
+        <v>1</v>
+      </c>
+      <c r="L282" t="n">
+        <v>30</v>
+      </c>
+      <c r="M282" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="283">
+      <c r="A283" t="inlineStr">
+        <is>
+          <t>Afsar Khan</t>
+        </is>
+      </c>
+      <c r="B283" t="inlineStr">
+        <is>
+          <t>REDX_VMS Portal</t>
+        </is>
+      </c>
+      <c r="C283" t="inlineStr">
+        <is>
+          <t>Mumbai Maharashtra India</t>
+        </is>
+      </c>
+      <c r="D283" t="inlineStr">
+        <is>
+          <t>Gosling</t>
+        </is>
+      </c>
+      <c r="E283" t="n">
+        <v>4.17</v>
+      </c>
+      <c r="F283" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="G283" t="inlineStr">
+        <is>
+          <t>Honeywell</t>
+        </is>
+      </c>
+      <c r="H283" t="inlineStr">
+        <is>
+          <t>5MP (2560x1920)</t>
+        </is>
+      </c>
+      <c r="I283" t="n">
+        <v>25</v>
+      </c>
+      <c r="J283" t="inlineStr">
+        <is>
+          <t>H265</t>
+        </is>
+      </c>
+      <c r="K283" t="n">
+        <v>1</v>
+      </c>
+      <c r="L283" t="n">
+        <v>30</v>
+      </c>
+      <c r="M283" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="284">
+      <c r="A284" t="inlineStr">
+        <is>
+          <t>Afsar Khan</t>
+        </is>
+      </c>
+      <c r="B284" t="inlineStr">
+        <is>
+          <t>REDX_VMS Portal</t>
+        </is>
+      </c>
+      <c r="C284" t="inlineStr">
+        <is>
+          <t>Mumbai Maharashtra India</t>
+        </is>
+      </c>
+      <c r="D284" t="inlineStr">
+        <is>
+          <t>Mr.Nitin</t>
+        </is>
+      </c>
+      <c r="E284" t="n">
+        <v>4.17</v>
+      </c>
+      <c r="F284" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="G284" t="inlineStr">
+        <is>
+          <t>Honeywell</t>
+        </is>
+      </c>
+      <c r="H284" t="inlineStr">
+        <is>
+          <t>5MP (2560x1920)</t>
+        </is>
+      </c>
+      <c r="I284" t="n">
+        <v>25</v>
+      </c>
+      <c r="J284" t="inlineStr">
+        <is>
+          <t>H265</t>
+        </is>
+      </c>
+      <c r="K284" t="n">
+        <v>1</v>
+      </c>
+      <c r="L284" t="n">
+        <v>30</v>
+      </c>
+      <c r="M284" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="285">
+      <c r="A285" t="inlineStr">
+        <is>
+          <t>Afsar Khan</t>
+        </is>
+      </c>
+      <c r="B285" t="inlineStr">
+        <is>
+          <t>REDX_VMS Portal</t>
+        </is>
+      </c>
+      <c r="C285" t="inlineStr">
+        <is>
+          <t>Mumbai Maharashtra India</t>
+        </is>
+      </c>
+      <c r="D285" t="inlineStr">
+        <is>
+          <t>Mr.Nitin</t>
+        </is>
+      </c>
+      <c r="E285" t="n">
+        <v>4.17</v>
+      </c>
+      <c r="F285" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="G285" t="inlineStr">
+        <is>
+          <t>Honeywell</t>
+        </is>
+      </c>
+      <c r="H285" t="inlineStr">
+        <is>
+          <t>5MP (2560x1920)</t>
+        </is>
+      </c>
+      <c r="I285" t="n">
+        <v>25</v>
+      </c>
+      <c r="J285" t="inlineStr">
+        <is>
+          <t>H265</t>
+        </is>
+      </c>
+      <c r="K285" t="n">
+        <v>1</v>
+      </c>
+      <c r="L285" t="n">
+        <v>30</v>
+      </c>
+      <c r="M285" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="286">
+      <c r="A286" t="inlineStr">
+        <is>
+          <t>Afsar Khan</t>
+        </is>
+      </c>
+      <c r="B286" t="inlineStr">
+        <is>
+          <t>REDX_VMS Portal</t>
+        </is>
+      </c>
+      <c r="C286" t="inlineStr">
+        <is>
+          <t>Mumbai Maharashtra India</t>
+        </is>
+      </c>
+      <c r="D286" t="inlineStr">
+        <is>
+          <t>Mr.Nitin</t>
+        </is>
+      </c>
+      <c r="E286" t="n">
+        <v>4.17</v>
+      </c>
+      <c r="F286" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="G286" t="inlineStr">
+        <is>
+          <t>Honeywell</t>
+        </is>
+      </c>
+      <c r="H286" t="inlineStr">
+        <is>
+          <t>5MP (2560x1920)</t>
+        </is>
+      </c>
+      <c r="I286" t="n">
+        <v>25</v>
+      </c>
+      <c r="J286" t="inlineStr">
+        <is>
+          <t>H265</t>
+        </is>
+      </c>
+      <c r="K286" t="n">
+        <v>1</v>
+      </c>
+      <c r="L286" t="n">
+        <v>30</v>
+      </c>
+      <c r="M286" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="287">
+      <c r="A287" t="inlineStr">
+        <is>
+          <t>Afsar Khan</t>
+        </is>
+      </c>
+      <c r="B287" t="inlineStr">
+        <is>
+          <t>REDX_VMS Portal</t>
+        </is>
+      </c>
+      <c r="C287" t="inlineStr">
+        <is>
+          <t>Mumbai Maharashtra India</t>
+        </is>
+      </c>
+      <c r="D287" t="inlineStr">
+        <is>
+          <t>Mr.Nitin</t>
+        </is>
+      </c>
+      <c r="E287" t="n">
+        <v>4.17</v>
+      </c>
+      <c r="F287" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="G287" t="inlineStr">
+        <is>
+          <t>Honeywell</t>
+        </is>
+      </c>
+      <c r="H287" t="inlineStr">
+        <is>
+          <t>5MP (2560x1920)</t>
+        </is>
+      </c>
+      <c r="I287" t="n">
+        <v>25</v>
+      </c>
+      <c r="J287" t="inlineStr">
+        <is>
+          <t>H265</t>
+        </is>
+      </c>
+      <c r="K287" t="n">
+        <v>1</v>
+      </c>
+      <c r="L287" t="n">
+        <v>30</v>
+      </c>
+      <c r="M287" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="288">
+      <c r="A288" t="inlineStr">
+        <is>
+          <t>Afsar Khan</t>
+        </is>
+      </c>
+      <c r="B288" t="inlineStr">
+        <is>
+          <t>REDX_VMS Portal</t>
+        </is>
+      </c>
+      <c r="C288" t="inlineStr">
+        <is>
+          <t>Mumbai Maharashtra India</t>
+        </is>
+      </c>
+      <c r="D288" t="inlineStr">
+        <is>
+          <t>Mr.Nitin</t>
+        </is>
+      </c>
+      <c r="E288" t="n">
+        <v>4.17</v>
+      </c>
+      <c r="F288" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="G288" t="inlineStr">
+        <is>
+          <t>Honeywell</t>
+        </is>
+      </c>
+      <c r="H288" t="inlineStr">
+        <is>
+          <t>5MP (2560x1920)</t>
+        </is>
+      </c>
+      <c r="I288" t="n">
+        <v>25</v>
+      </c>
+      <c r="J288" t="inlineStr">
+        <is>
+          <t>H265</t>
+        </is>
+      </c>
+      <c r="K288" t="n">
+        <v>1</v>
+      </c>
+      <c r="L288" t="n">
+        <v>30</v>
+      </c>
+      <c r="M288" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="289">
+      <c r="A289" t="inlineStr">
+        <is>
+          <t>Afsar Khan</t>
+        </is>
+      </c>
+      <c r="B289" t="inlineStr">
+        <is>
+          <t>REDX_VMS Portal</t>
+        </is>
+      </c>
+      <c r="C289" t="inlineStr">
+        <is>
+          <t>Mumbai Maharashtra India</t>
+        </is>
+      </c>
+      <c r="D289" t="inlineStr">
+        <is>
+          <t>Mr.Nitin</t>
+        </is>
+      </c>
+      <c r="E289" t="n">
+        <v>4.17</v>
+      </c>
+      <c r="F289" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="G289" t="inlineStr">
+        <is>
+          <t>Honeywell</t>
+        </is>
+      </c>
+      <c r="H289" t="inlineStr">
+        <is>
+          <t>5MP (2560x1920)</t>
+        </is>
+      </c>
+      <c r="I289" t="n">
+        <v>25</v>
+      </c>
+      <c r="J289" t="inlineStr">
+        <is>
+          <t>H265</t>
+        </is>
+      </c>
+      <c r="K289" t="n">
+        <v>1</v>
+      </c>
+      <c r="L289" t="n">
+        <v>30</v>
+      </c>
+      <c r="M289" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="290">
+      <c r="A290" t="inlineStr">
+        <is>
+          <t>Afsar Khan</t>
+        </is>
+      </c>
+      <c r="B290" t="inlineStr">
+        <is>
+          <t>REDX_VMS Portal</t>
+        </is>
+      </c>
+      <c r="C290" t="inlineStr">
+        <is>
+          <t>Mumbai Maharashtra India</t>
+        </is>
+      </c>
+      <c r="D290" t="inlineStr">
+        <is>
+          <t>Mr.Nitin</t>
+        </is>
+      </c>
+      <c r="E290" t="n">
+        <v>4.17</v>
+      </c>
+      <c r="F290" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="G290" t="inlineStr">
+        <is>
+          <t>Honeywell</t>
+        </is>
+      </c>
+      <c r="H290" t="inlineStr">
+        <is>
+          <t>5MP (2560x1920)</t>
+        </is>
+      </c>
+      <c r="I290" t="n">
+        <v>25</v>
+      </c>
+      <c r="J290" t="inlineStr">
+        <is>
+          <t>H265</t>
+        </is>
+      </c>
+      <c r="K290" t="n">
+        <v>1</v>
+      </c>
+      <c r="L290" t="n">
+        <v>30</v>
+      </c>
+      <c r="M290" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="291">
+      <c r="A291" t="inlineStr">
+        <is>
+          <t>Afsar Khan</t>
+        </is>
+      </c>
+      <c r="B291" t="inlineStr">
+        <is>
+          <t>REDX_VMS Portal</t>
+        </is>
+      </c>
+      <c r="C291" t="inlineStr">
+        <is>
+          <t>Mumbai Maharashtra India</t>
+        </is>
+      </c>
+      <c r="D291" t="inlineStr">
+        <is>
+          <t>Mr.Nitin</t>
+        </is>
+      </c>
+      <c r="E291" t="n">
+        <v>4.17</v>
+      </c>
+      <c r="F291" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="G291" t="inlineStr">
+        <is>
+          <t>Honeywell</t>
+        </is>
+      </c>
+      <c r="H291" t="inlineStr">
+        <is>
+          <t>5MP (2560x1920)</t>
+        </is>
+      </c>
+      <c r="I291" t="n">
+        <v>25</v>
+      </c>
+      <c r="J291" t="inlineStr">
+        <is>
+          <t>H265</t>
+        </is>
+      </c>
+      <c r="K291" t="n">
+        <v>1</v>
+      </c>
+      <c r="L291" t="n">
+        <v>30</v>
+      </c>
+      <c r="M291" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="292">
+      <c r="A292" t="inlineStr">
+        <is>
+          <t>Afsar Khan</t>
+        </is>
+      </c>
+      <c r="B292" t="inlineStr">
+        <is>
+          <t>REDX_VMS Portal</t>
+        </is>
+      </c>
+      <c r="C292" t="inlineStr">
+        <is>
+          <t>Mumbai Maharashtra India</t>
+        </is>
+      </c>
+      <c r="D292" t="inlineStr">
+        <is>
+          <t>Mr.Nitin</t>
+        </is>
+      </c>
+      <c r="E292" t="n">
+        <v>4.17</v>
+      </c>
+      <c r="F292" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="G292" t="inlineStr">
+        <is>
+          <t>Honeywell</t>
+        </is>
+      </c>
+      <c r="H292" t="inlineStr">
+        <is>
+          <t>5MP (2560x1920)</t>
+        </is>
+      </c>
+      <c r="I292" t="n">
+        <v>25</v>
+      </c>
+      <c r="J292" t="inlineStr">
+        <is>
+          <t>H265</t>
+        </is>
+      </c>
+      <c r="K292" t="n">
+        <v>1</v>
+      </c>
+      <c r="L292" t="n">
+        <v>30</v>
+      </c>
+      <c r="M292" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="293">
+      <c r="A293" t="inlineStr">
+        <is>
+          <t>Afsar Khan</t>
+        </is>
+      </c>
+      <c r="B293" t="inlineStr">
+        <is>
+          <t>REDX_VMS Portal</t>
+        </is>
+      </c>
+      <c r="C293" t="inlineStr">
+        <is>
+          <t>Mumbai Maharashtra India</t>
+        </is>
+      </c>
+      <c r="D293" t="inlineStr">
+        <is>
+          <t>Mr.Nitin</t>
+        </is>
+      </c>
+      <c r="E293" t="n">
+        <v>4.17</v>
+      </c>
+      <c r="F293" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="G293" t="inlineStr">
+        <is>
+          <t>Honeywell</t>
+        </is>
+      </c>
+      <c r="H293" t="inlineStr">
+        <is>
+          <t>5MP (2560x1920)</t>
+        </is>
+      </c>
+      <c r="I293" t="n">
+        <v>25</v>
+      </c>
+      <c r="J293" t="inlineStr">
+        <is>
+          <t>H265</t>
+        </is>
+      </c>
+      <c r="K293" t="n">
+        <v>1</v>
+      </c>
+      <c r="L293" t="n">
+        <v>30</v>
+      </c>
+      <c r="M293" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="294">
+      <c r="A294" t="inlineStr">
+        <is>
+          <t>Afsar Khan</t>
+        </is>
+      </c>
+      <c r="B294" t="inlineStr">
+        <is>
+          <t>REDX_VMS Portal</t>
+        </is>
+      </c>
+      <c r="C294" t="inlineStr">
+        <is>
+          <t>Mumbai Maharashtra India</t>
+        </is>
+      </c>
+      <c r="D294" t="inlineStr">
+        <is>
+          <t>Mr.Nitin</t>
+        </is>
+      </c>
+      <c r="E294" t="n">
+        <v>4.17</v>
+      </c>
+      <c r="F294" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="G294" t="inlineStr">
+        <is>
+          <t>Honeywell</t>
+        </is>
+      </c>
+      <c r="H294" t="inlineStr">
+        <is>
+          <t>5MP (2560x1920)</t>
+        </is>
+      </c>
+      <c r="I294" t="n">
+        <v>25</v>
+      </c>
+      <c r="J294" t="inlineStr">
+        <is>
+          <t>H265</t>
+        </is>
+      </c>
+      <c r="K294" t="n">
+        <v>1</v>
+      </c>
+      <c r="L294" t="n">
+        <v>30</v>
+      </c>
+      <c r="M294" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="295">
+      <c r="A295" t="inlineStr">
+        <is>
+          <t>Afsar Khan</t>
+        </is>
+      </c>
+      <c r="B295" t="inlineStr">
+        <is>
+          <t>REDX_VMS Portal</t>
+        </is>
+      </c>
+      <c r="C295" t="inlineStr">
+        <is>
+          <t>Mumbai Maharashtra India</t>
+        </is>
+      </c>
+      <c r="D295" t="inlineStr">
+        <is>
+          <t>Mr.Nitin</t>
+        </is>
+      </c>
+      <c r="E295" t="n">
+        <v>4.17</v>
+      </c>
+      <c r="F295" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="G295" t="inlineStr">
+        <is>
+          <t>Honeywell</t>
+        </is>
+      </c>
+      <c r="H295" t="inlineStr">
+        <is>
+          <t>5MP (2560x1920)</t>
+        </is>
+      </c>
+      <c r="I295" t="n">
+        <v>25</v>
+      </c>
+      <c r="J295" t="inlineStr">
+        <is>
+          <t>H265</t>
+        </is>
+      </c>
+      <c r="K295" t="n">
+        <v>1</v>
+      </c>
+      <c r="L295" t="n">
+        <v>30</v>
+      </c>
+      <c r="M295" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="296">
+      <c r="A296" t="inlineStr">
+        <is>
+          <t>Afsar Khan</t>
+        </is>
+      </c>
+      <c r="B296" t="inlineStr">
+        <is>
+          <t>REDX_VMS Portal</t>
+        </is>
+      </c>
+      <c r="C296" t="inlineStr">
+        <is>
+          <t>Mumbai Maharashtra India</t>
+        </is>
+      </c>
+      <c r="D296" t="inlineStr">
+        <is>
+          <t>Mr.Nitin</t>
+        </is>
+      </c>
+      <c r="E296" t="n">
+        <v>4.17</v>
+      </c>
+      <c r="F296" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="G296" t="inlineStr">
+        <is>
+          <t>Honeywell</t>
+        </is>
+      </c>
+      <c r="H296" t="inlineStr">
+        <is>
+          <t>5MP (2560x1920)</t>
+        </is>
+      </c>
+      <c r="I296" t="n">
+        <v>25</v>
+      </c>
+      <c r="J296" t="inlineStr">
+        <is>
+          <t>H265</t>
+        </is>
+      </c>
+      <c r="K296" t="n">
+        <v>1</v>
+      </c>
+      <c r="L296" t="n">
+        <v>30</v>
+      </c>
+      <c r="M296" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="297">
+      <c r="A297" t="inlineStr">
+        <is>
+          <t>Afsar Khan</t>
+        </is>
+      </c>
+      <c r="B297" t="inlineStr">
+        <is>
+          <t>REDX_VMS Portal</t>
+        </is>
+      </c>
+      <c r="C297" t="inlineStr">
+        <is>
+          <t>Mumbai Maharashtra India</t>
+        </is>
+      </c>
+      <c r="D297" t="inlineStr">
+        <is>
+          <t>Mr.Nitin</t>
+        </is>
+      </c>
+      <c r="E297" t="n">
+        <v>4.17</v>
+      </c>
+      <c r="F297" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="G297" t="inlineStr">
+        <is>
+          <t>Honeywell</t>
+        </is>
+      </c>
+      <c r="H297" t="inlineStr">
+        <is>
+          <t>5MP (2560x1920)</t>
+        </is>
+      </c>
+      <c r="I297" t="n">
+        <v>25</v>
+      </c>
+      <c r="J297" t="inlineStr">
+        <is>
+          <t>H265</t>
+        </is>
+      </c>
+      <c r="K297" t="n">
+        <v>1</v>
+      </c>
+      <c r="L297" t="n">
+        <v>30</v>
+      </c>
+      <c r="M297" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="298">
+      <c r="A298" t="inlineStr">
+        <is>
+          <t>Afsar Khan</t>
+        </is>
+      </c>
+      <c r="B298" t="inlineStr">
+        <is>
+          <t>REDX_VMS Portal</t>
+        </is>
+      </c>
+      <c r="C298" t="inlineStr">
+        <is>
+          <t>Mumbai Maharashtra India</t>
+        </is>
+      </c>
+      <c r="D298" t="inlineStr">
+        <is>
+          <t>Mr.Nitin</t>
+        </is>
+      </c>
+      <c r="E298" t="n">
+        <v>4.17</v>
+      </c>
+      <c r="F298" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="G298" t="inlineStr">
+        <is>
+          <t>Honeywell</t>
+        </is>
+      </c>
+      <c r="H298" t="inlineStr">
+        <is>
+          <t>5MP (2560x1920)</t>
+        </is>
+      </c>
+      <c r="I298" t="n">
+        <v>25</v>
+      </c>
+      <c r="J298" t="inlineStr">
+        <is>
+          <t>H265</t>
+        </is>
+      </c>
+      <c r="K298" t="n">
+        <v>1</v>
+      </c>
+      <c r="L298" t="n">
+        <v>30</v>
+      </c>
+      <c r="M298" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="299">
+      <c r="A299" t="inlineStr">
+        <is>
+          <t>Afsar Khan</t>
+        </is>
+      </c>
+      <c r="B299" t="inlineStr">
+        <is>
+          <t>REDX_VMS Portal</t>
+        </is>
+      </c>
+      <c r="C299" t="inlineStr">
+        <is>
+          <t>Mumbai Maharashtra India</t>
+        </is>
+      </c>
+      <c r="D299" t="inlineStr">
+        <is>
+          <t>Mr.Nitin</t>
+        </is>
+      </c>
+      <c r="E299" t="n">
+        <v>4.17</v>
+      </c>
+      <c r="F299" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="G299" t="inlineStr">
+        <is>
+          <t>Honeywell</t>
+        </is>
+      </c>
+      <c r="H299" t="inlineStr">
+        <is>
+          <t>5MP (2560x1920)</t>
+        </is>
+      </c>
+      <c r="I299" t="n">
+        <v>25</v>
+      </c>
+      <c r="J299" t="inlineStr">
+        <is>
+          <t>H265</t>
+        </is>
+      </c>
+      <c r="K299" t="n">
+        <v>1</v>
+      </c>
+      <c r="L299" t="n">
+        <v>30</v>
+      </c>
+      <c r="M299" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="300">
+      <c r="A300" t="inlineStr">
+        <is>
+          <t>Afsar Khan</t>
+        </is>
+      </c>
+      <c r="B300" t="inlineStr">
+        <is>
+          <t>REDX_VMS Portal</t>
+        </is>
+      </c>
+      <c r="C300" t="inlineStr">
+        <is>
+          <t>Mumbai Maharashtra India</t>
+        </is>
+      </c>
+      <c r="D300" t="inlineStr">
+        <is>
+          <t>Mr.Nitin</t>
+        </is>
+      </c>
+      <c r="E300" t="n">
+        <v>4.17</v>
+      </c>
+      <c r="F300" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="G300" t="inlineStr">
+        <is>
+          <t>Honeywell</t>
+        </is>
+      </c>
+      <c r="H300" t="inlineStr">
+        <is>
+          <t>5MP (2560x1920)</t>
+        </is>
+      </c>
+      <c r="I300" t="n">
+        <v>25</v>
+      </c>
+      <c r="J300" t="inlineStr">
+        <is>
+          <t>H265</t>
+        </is>
+      </c>
+      <c r="K300" t="n">
+        <v>1</v>
+      </c>
+      <c r="L300" t="n">
+        <v>30</v>
+      </c>
+      <c r="M300" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="301">
+      <c r="A301" t="inlineStr">
+        <is>
+          <t>Afsar Khan</t>
+        </is>
+      </c>
+      <c r="B301" t="inlineStr">
+        <is>
+          <t>REDX_VMS Portal</t>
+        </is>
+      </c>
+      <c r="C301" t="inlineStr">
+        <is>
+          <t>Mumbai Maharashtra India</t>
+        </is>
+      </c>
+      <c r="D301" t="inlineStr">
+        <is>
+          <t>Mr.Nitin</t>
+        </is>
+      </c>
+      <c r="E301" t="n">
+        <v>4.17</v>
+      </c>
+      <c r="F301" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="G301" t="inlineStr">
+        <is>
+          <t>Honeywell</t>
+        </is>
+      </c>
+      <c r="H301" t="inlineStr">
+        <is>
+          <t>5MP (2560x1920)</t>
+        </is>
+      </c>
+      <c r="I301" t="n">
+        <v>25</v>
+      </c>
+      <c r="J301" t="inlineStr">
+        <is>
+          <t>H265</t>
+        </is>
+      </c>
+      <c r="K301" t="n">
+        <v>1</v>
+      </c>
+      <c r="L301" t="n">
+        <v>30</v>
+      </c>
+      <c r="M301" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>Afsar Khan</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>REDX_VMS Portal</t>
+        </is>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>Mumbai Maharashtra India</t>
+        </is>
+      </c>
+      <c r="D302" t="inlineStr">
+        <is>
+          <t>Mr.Nitin</t>
+        </is>
+      </c>
+      <c r="E302" t="n">
+        <v>4.17</v>
+      </c>
+      <c r="F302" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="G302" t="inlineStr">
+        <is>
+          <t>Honeywell</t>
+        </is>
+      </c>
+      <c r="H302" t="inlineStr">
+        <is>
+          <t>5MP (2560x1920)</t>
+        </is>
+      </c>
+      <c r="I302" t="n">
+        <v>25</v>
+      </c>
+      <c r="J302" t="inlineStr">
+        <is>
+          <t>H265</t>
+        </is>
+      </c>
+      <c r="K302" t="n">
+        <v>1</v>
+      </c>
+      <c r="L302" t="n">
+        <v>30</v>
+      </c>
+      <c r="M302" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>Afsar Khan</t>
+        </is>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>REDX_VMS Portal</t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>Mumbai Maharashtra India</t>
+        </is>
+      </c>
+      <c r="D303" t="inlineStr">
+        <is>
+          <t>Mr.Nitin</t>
+        </is>
+      </c>
+      <c r="E303" t="n">
+        <v>4.17</v>
+      </c>
+      <c r="F303" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="G303" t="inlineStr">
+        <is>
+          <t>Honeywell</t>
+        </is>
+      </c>
+      <c r="H303" t="inlineStr">
+        <is>
+          <t>5MP (2560x1920)</t>
+        </is>
+      </c>
+      <c r="I303" t="n">
+        <v>25</v>
+      </c>
+      <c r="J303" t="inlineStr">
+        <is>
+          <t>H265</t>
+        </is>
+      </c>
+      <c r="K303" t="n">
+        <v>1</v>
+      </c>
+      <c r="L303" t="n">
+        <v>30</v>
+      </c>
+      <c r="M303" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>Afsar Khan</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>REDX_VMS Portal</t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>Mumbai Maharashtra India</t>
+        </is>
+      </c>
+      <c r="D304" t="inlineStr">
+        <is>
+          <t>Mr.Nitin</t>
+        </is>
+      </c>
+      <c r="E304" t="n">
+        <v>4.17</v>
+      </c>
+      <c r="F304" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="G304" t="inlineStr">
+        <is>
+          <t>Honeywell</t>
+        </is>
+      </c>
+      <c r="H304" t="inlineStr">
+        <is>
+          <t>5MP (2560x1920)</t>
+        </is>
+      </c>
+      <c r="I304" t="n">
+        <v>25</v>
+      </c>
+      <c r="J304" t="inlineStr">
+        <is>
+          <t>H265</t>
+        </is>
+      </c>
+      <c r="K304" t="n">
+        <v>1</v>
+      </c>
+      <c r="L304" t="n">
+        <v>30</v>
+      </c>
+      <c r="M304" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>Afsar Khan</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>REDX_VMS Portal</t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>Mumbai Maharashtra India</t>
+        </is>
+      </c>
+      <c r="D305" t="inlineStr">
+        <is>
+          <t>Mr.Nitin</t>
+        </is>
+      </c>
+      <c r="E305" t="n">
+        <v>4.17</v>
+      </c>
+      <c r="F305" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="G305" t="inlineStr">
+        <is>
+          <t>Honeywell</t>
+        </is>
+      </c>
+      <c r="H305" t="inlineStr">
+        <is>
+          <t>5MP (2560x1920)</t>
+        </is>
+      </c>
+      <c r="I305" t="n">
+        <v>25</v>
+      </c>
+      <c r="J305" t="inlineStr">
+        <is>
+          <t>H265</t>
+        </is>
+      </c>
+      <c r="K305" t="n">
+        <v>1</v>
+      </c>
+      <c r="L305" t="n">
+        <v>30</v>
+      </c>
+      <c r="M305" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>Afsar Khan</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>REDX_VMS Portal</t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>Mumbai Maharashtra India</t>
+        </is>
+      </c>
+      <c r="D306" t="inlineStr">
+        <is>
+          <t>Mr.Nitin</t>
+        </is>
+      </c>
+      <c r="E306" t="n">
+        <v>4.17</v>
+      </c>
+      <c r="F306" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="G306" t="inlineStr">
+        <is>
+          <t>Honeywell</t>
+        </is>
+      </c>
+      <c r="H306" t="inlineStr">
+        <is>
+          <t>5MP (2560x1920)</t>
+        </is>
+      </c>
+      <c r="I306" t="n">
+        <v>25</v>
+      </c>
+      <c r="J306" t="inlineStr">
+        <is>
+          <t>H265</t>
+        </is>
+      </c>
+      <c r="K306" t="n">
+        <v>1</v>
+      </c>
+      <c r="L306" t="n">
+        <v>30</v>
+      </c>
+      <c r="M306" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>Afsar Khan</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>REDX_VMS Portal</t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>Mumbai Maharashtra India</t>
+        </is>
+      </c>
+      <c r="D307" t="inlineStr">
+        <is>
+          <t>Mr.Nitin</t>
+        </is>
+      </c>
+      <c r="E307" t="n">
+        <v>4.17</v>
+      </c>
+      <c r="F307" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="G307" t="inlineStr">
+        <is>
+          <t>Honeywell</t>
+        </is>
+      </c>
+      <c r="H307" t="inlineStr">
+        <is>
+          <t>5MP (2560x1920)</t>
+        </is>
+      </c>
+      <c r="I307" t="n">
+        <v>25</v>
+      </c>
+      <c r="J307" t="inlineStr">
+        <is>
+          <t>H265</t>
+        </is>
+      </c>
+      <c r="K307" t="n">
+        <v>1</v>
+      </c>
+      <c r="L307" t="n">
+        <v>30</v>
+      </c>
+      <c r="M307" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>Afsar Khan</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>REDX_VMS Portal</t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>Mumbai Maharashtra India</t>
+        </is>
+      </c>
+      <c r="D308" t="inlineStr">
+        <is>
+          <t>Mr.Nitin</t>
+        </is>
+      </c>
+      <c r="E308" t="n">
+        <v>4.17</v>
+      </c>
+      <c r="F308" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="G308" t="inlineStr">
+        <is>
+          <t>Honeywell</t>
+        </is>
+      </c>
+      <c r="H308" t="inlineStr">
+        <is>
+          <t>5MP (2560x1920)</t>
+        </is>
+      </c>
+      <c r="I308" t="n">
+        <v>25</v>
+      </c>
+      <c r="J308" t="inlineStr">
+        <is>
+          <t>H265</t>
+        </is>
+      </c>
+      <c r="K308" t="n">
+        <v>1</v>
+      </c>
+      <c r="L308" t="n">
+        <v>30</v>
+      </c>
+      <c r="M308" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>Afsar Khan</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>REDX_VMS Portal</t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>Mumbai Maharashtra India</t>
+        </is>
+      </c>
+      <c r="D309" t="inlineStr">
+        <is>
+          <t>Mr.Nitin</t>
+        </is>
+      </c>
+      <c r="E309" t="n">
+        <v>4.17</v>
+      </c>
+      <c r="F309" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="G309" t="inlineStr">
+        <is>
+          <t>Honeywell</t>
+        </is>
+      </c>
+      <c r="H309" t="inlineStr">
+        <is>
+          <t>5MP (2560x1920)</t>
+        </is>
+      </c>
+      <c r="I309" t="n">
+        <v>25</v>
+      </c>
+      <c r="J309" t="inlineStr">
+        <is>
+          <t>H265</t>
+        </is>
+      </c>
+      <c r="K309" t="n">
+        <v>1</v>
+      </c>
+      <c r="L309" t="n">
+        <v>30</v>
+      </c>
+      <c r="M309" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>Afsar Khan</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>REDX_VMS Portal</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>Mumbai Maharashtra India</t>
+        </is>
+      </c>
+      <c r="D310" t="inlineStr">
+        <is>
+          <t>Mr.Nitin</t>
+        </is>
+      </c>
+      <c r="E310" t="n">
+        <v>4.17</v>
+      </c>
+      <c r="F310" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="G310" t="inlineStr">
+        <is>
+          <t>Honeywell</t>
+        </is>
+      </c>
+      <c r="H310" t="inlineStr">
+        <is>
+          <t>5MP (2560x1920)</t>
+        </is>
+      </c>
+      <c r="I310" t="n">
+        <v>25</v>
+      </c>
+      <c r="J310" t="inlineStr">
+        <is>
+          <t>H265</t>
+        </is>
+      </c>
+      <c r="K310" t="n">
+        <v>1</v>
+      </c>
+      <c r="L310" t="n">
+        <v>30</v>
+      </c>
+      <c r="M310" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>Afsar Khan</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>REDX_VMS Portal</t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>Mumbai Maharashtra India</t>
+        </is>
+      </c>
+      <c r="D311" t="inlineStr">
+        <is>
+          <t>Mr.Nitin</t>
+        </is>
+      </c>
+      <c r="E311" t="n">
+        <v>4.17</v>
+      </c>
+      <c r="F311" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="G311" t="inlineStr">
+        <is>
+          <t>Honeywell</t>
+        </is>
+      </c>
+      <c r="H311" t="inlineStr">
+        <is>
+          <t>5MP (2560x1920)</t>
+        </is>
+      </c>
+      <c r="I311" t="n">
+        <v>25</v>
+      </c>
+      <c r="J311" t="inlineStr">
+        <is>
+          <t>H265</t>
+        </is>
+      </c>
+      <c r="K311" t="n">
+        <v>1</v>
+      </c>
+      <c r="L311" t="n">
+        <v>30</v>
+      </c>
+      <c r="M311" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>Afsar Khan</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>REDX_VMS Portal</t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>Mumbai Maharashtra India</t>
+        </is>
+      </c>
+      <c r="D312" t="inlineStr">
+        <is>
+          <t>Mr.Nitin</t>
+        </is>
+      </c>
+      <c r="E312" t="n">
+        <v>4.17</v>
+      </c>
+      <c r="F312" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="G312" t="inlineStr">
+        <is>
+          <t>Honeywell</t>
+        </is>
+      </c>
+      <c r="H312" t="inlineStr">
+        <is>
+          <t>5MP (2560x1920)</t>
+        </is>
+      </c>
+      <c r="I312" t="n">
+        <v>25</v>
+      </c>
+      <c r="J312" t="inlineStr">
+        <is>
+          <t>H265</t>
+        </is>
+      </c>
+      <c r="K312" t="n">
+        <v>1</v>
+      </c>
+      <c r="L312" t="n">
+        <v>30</v>
+      </c>
+      <c r="M312" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>Afsar Khan</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>REDX_VMS Portal</t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>Mumbai Maharashtra India</t>
+        </is>
+      </c>
+      <c r="D313" t="inlineStr">
+        <is>
+          <t>Mr.Nitin</t>
+        </is>
+      </c>
+      <c r="E313" t="n">
+        <v>4.17</v>
+      </c>
+      <c r="F313" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="G313" t="inlineStr">
+        <is>
+          <t>Honeywell</t>
+        </is>
+      </c>
+      <c r="H313" t="inlineStr">
+        <is>
+          <t>5MP (2560x1920)</t>
+        </is>
+      </c>
+      <c r="I313" t="n">
+        <v>25</v>
+      </c>
+      <c r="J313" t="inlineStr">
+        <is>
+          <t>H265</t>
+        </is>
+      </c>
+      <c r="K313" t="n">
+        <v>1</v>
+      </c>
+      <c r="L313" t="n">
+        <v>30</v>
+      </c>
+      <c r="M313" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>Afsar Khan</t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>REDX_VMS Portal</t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>Mumbai Maharashtra India</t>
+        </is>
+      </c>
+      <c r="D314" t="inlineStr">
+        <is>
+          <t>Mr.Nitin</t>
+        </is>
+      </c>
+      <c r="E314" t="n">
+        <v>4.17</v>
+      </c>
+      <c r="F314" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="G314" t="inlineStr">
+        <is>
+          <t>Honeywell</t>
+        </is>
+      </c>
+      <c r="H314" t="inlineStr">
+        <is>
+          <t>5MP (2560x1920)</t>
+        </is>
+      </c>
+      <c r="I314" t="n">
+        <v>25</v>
+      </c>
+      <c r="J314" t="inlineStr">
+        <is>
+          <t>H265</t>
+        </is>
+      </c>
+      <c r="K314" t="n">
+        <v>1</v>
+      </c>
+      <c r="L314" t="n">
+        <v>30</v>
+      </c>
+      <c r="M314" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>Afsar Khan</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>REDX_VMS Portal</t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>Mumbai Maharashtra India</t>
+        </is>
+      </c>
+      <c r="D315" t="inlineStr">
+        <is>
+          <t>Mr.Nitin</t>
+        </is>
+      </c>
+      <c r="E315" t="n">
+        <v>4.17</v>
+      </c>
+      <c r="F315" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="G315" t="inlineStr">
+        <is>
+          <t>Honeywell</t>
+        </is>
+      </c>
+      <c r="H315" t="inlineStr">
+        <is>
+          <t>5MP (2560x1920)</t>
+        </is>
+      </c>
+      <c r="I315" t="n">
+        <v>25</v>
+      </c>
+      <c r="J315" t="inlineStr">
+        <is>
+          <t>H265</t>
+        </is>
+      </c>
+      <c r="K315" t="n">
+        <v>1</v>
+      </c>
+      <c r="L315" t="n">
+        <v>30</v>
+      </c>
+      <c r="M315" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>Afsar Khan</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>REDX_VMS Portal</t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>Mumbai Maharashtra India</t>
+        </is>
+      </c>
+      <c r="D316" t="inlineStr">
+        <is>
+          <t>Mr.Nitin</t>
+        </is>
+      </c>
+      <c r="E316" t="n">
+        <v>4.17</v>
+      </c>
+      <c r="F316" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="G316" t="inlineStr">
+        <is>
+          <t>Honeywell</t>
+        </is>
+      </c>
+      <c r="H316" t="inlineStr">
+        <is>
+          <t>5MP (2560x1920)</t>
+        </is>
+      </c>
+      <c r="I316" t="n">
+        <v>25</v>
+      </c>
+      <c r="J316" t="inlineStr">
+        <is>
+          <t>H265</t>
+        </is>
+      </c>
+      <c r="K316" t="n">
+        <v>1</v>
+      </c>
+      <c r="L316" t="n">
+        <v>30</v>
+      </c>
+      <c r="M316" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>Afsar Khan</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>REDX_VMS Portal</t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>Mumbai Maharashtra India</t>
+        </is>
+      </c>
+      <c r="D317" t="inlineStr">
+        <is>
+          <t>Mr.Nitin</t>
+        </is>
+      </c>
+      <c r="E317" t="n">
+        <v>4.17</v>
+      </c>
+      <c r="F317" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="G317" t="inlineStr">
+        <is>
+          <t>Honeywell</t>
+        </is>
+      </c>
+      <c r="H317" t="inlineStr">
+        <is>
+          <t>5MP (2560x1920)</t>
+        </is>
+      </c>
+      <c r="I317" t="n">
+        <v>25</v>
+      </c>
+      <c r="J317" t="inlineStr">
+        <is>
+          <t>H265</t>
+        </is>
+      </c>
+      <c r="K317" t="n">
+        <v>1</v>
+      </c>
+      <c r="L317" t="n">
+        <v>30</v>
+      </c>
+      <c r="M317" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>Afsar Khan</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>REDX_VMS Portal</t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>Mumbai Maharashtra India</t>
+        </is>
+      </c>
+      <c r="D318" t="inlineStr">
+        <is>
+          <t>Mr.Nitin</t>
+        </is>
+      </c>
+      <c r="E318" t="n">
+        <v>4.17</v>
+      </c>
+      <c r="F318" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="G318" t="inlineStr">
+        <is>
+          <t>Honeywell</t>
+        </is>
+      </c>
+      <c r="H318" t="inlineStr">
+        <is>
+          <t>5MP (2560x1920)</t>
+        </is>
+      </c>
+      <c r="I318" t="n">
+        <v>25</v>
+      </c>
+      <c r="J318" t="inlineStr">
+        <is>
+          <t>H265</t>
+        </is>
+      </c>
+      <c r="K318" t="n">
+        <v>1</v>
+      </c>
+      <c r="L318" t="n">
+        <v>30</v>
+      </c>
+      <c r="M318" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>Afsar Khan</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>REDX_VMS Portal</t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>Mumbai Maharashtra India</t>
+        </is>
+      </c>
+      <c r="D319" t="inlineStr">
+        <is>
+          <t>Mr.Nitin</t>
+        </is>
+      </c>
+      <c r="E319" t="n">
+        <v>4.17</v>
+      </c>
+      <c r="F319" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="G319" t="inlineStr">
+        <is>
+          <t>Honeywell</t>
+        </is>
+      </c>
+      <c r="H319" t="inlineStr">
+        <is>
+          <t>5MP (2560x1920)</t>
+        </is>
+      </c>
+      <c r="I319" t="n">
+        <v>25</v>
+      </c>
+      <c r="J319" t="inlineStr">
+        <is>
+          <t>H265</t>
+        </is>
+      </c>
+      <c r="K319" t="n">
+        <v>1</v>
+      </c>
+      <c r="L319" t="n">
+        <v>30</v>
+      </c>
+      <c r="M319" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>Afsar Khan</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>REDX_VMS Portal</t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>Mumbai Maharashtra India</t>
+        </is>
+      </c>
+      <c r="D320" t="inlineStr">
+        <is>
+          <t>Mr.Nitin</t>
+        </is>
+      </c>
+      <c r="E320" t="n">
+        <v>4.17</v>
+      </c>
+      <c r="F320" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="G320" t="inlineStr">
+        <is>
+          <t>Honeywell</t>
+        </is>
+      </c>
+      <c r="H320" t="inlineStr">
+        <is>
+          <t>5MP (2560x1920)</t>
+        </is>
+      </c>
+      <c r="I320" t="n">
+        <v>25</v>
+      </c>
+      <c r="J320" t="inlineStr">
+        <is>
+          <t>H265</t>
+        </is>
+      </c>
+      <c r="K320" t="n">
+        <v>1</v>
+      </c>
+      <c r="L320" t="n">
+        <v>30</v>
+      </c>
+      <c r="M320" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>Afsar Khan</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>REDX_VMS Portal</t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>Mumbai Maharashtra India</t>
+        </is>
+      </c>
+      <c r="D321" t="inlineStr">
+        <is>
+          <t>Mr.Nitin</t>
+        </is>
+      </c>
+      <c r="E321" t="n">
+        <v>4.17</v>
+      </c>
+      <c r="F321" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="G321" t="inlineStr">
+        <is>
+          <t>Honeywell</t>
+        </is>
+      </c>
+      <c r="H321" t="inlineStr">
+        <is>
+          <t>5MP (2560x1920)</t>
+        </is>
+      </c>
+      <c r="I321" t="n">
+        <v>25</v>
+      </c>
+      <c r="J321" t="inlineStr">
+        <is>
+          <t>H265</t>
+        </is>
+      </c>
+      <c r="K321" t="n">
+        <v>1</v>
+      </c>
+      <c r="L321" t="n">
+        <v>30</v>
+      </c>
+      <c r="M321" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>Afsar Khan</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>REDX_VMS Portal</t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>Mumbai Maharashtra India</t>
+        </is>
+      </c>
+      <c r="D322" t="inlineStr">
+        <is>
+          <t>Mr.Nitin</t>
+        </is>
+      </c>
+      <c r="E322" t="n">
+        <v>4.17</v>
+      </c>
+      <c r="F322" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="G322" t="inlineStr">
+        <is>
+          <t>Honeywell</t>
+        </is>
+      </c>
+      <c r="H322" t="inlineStr">
+        <is>
+          <t>5MP (2560x1920)</t>
+        </is>
+      </c>
+      <c r="I322" t="n">
+        <v>25</v>
+      </c>
+      <c r="J322" t="inlineStr">
+        <is>
+          <t>H265</t>
+        </is>
+      </c>
+      <c r="K322" t="n">
+        <v>1</v>
+      </c>
+      <c r="L322" t="n">
+        <v>30</v>
+      </c>
+      <c r="M322" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>Afsar Khan</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>REDX_VMS Portal</t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>Mumbai Maharashtra India</t>
+        </is>
+      </c>
+      <c r="D323" t="inlineStr">
+        <is>
+          <t>Mr.Nitin</t>
+        </is>
+      </c>
+      <c r="E323" t="n">
+        <v>4.17</v>
+      </c>
+      <c r="F323" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="G323" t="inlineStr">
+        <is>
+          <t>Honeywell</t>
+        </is>
+      </c>
+      <c r="H323" t="inlineStr">
+        <is>
+          <t>5MP (2560x1920)</t>
+        </is>
+      </c>
+      <c r="I323" t="n">
+        <v>25</v>
+      </c>
+      <c r="J323" t="inlineStr">
+        <is>
+          <t>H265</t>
+        </is>
+      </c>
+      <c r="K323" t="n">
+        <v>1</v>
+      </c>
+      <c r="L323" t="n">
+        <v>30</v>
+      </c>
+      <c r="M323" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>Afsar Khan</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>REDX_VMS Portal</t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>Mumbai Maharashtra India</t>
+        </is>
+      </c>
+      <c r="D324" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="E324" t="n">
+        <v>4.17</v>
+      </c>
+      <c r="F324" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="G324" t="inlineStr">
+        <is>
+          <t>Honeywell</t>
+        </is>
+      </c>
+      <c r="H324" t="inlineStr">
+        <is>
+          <t>5MP (2560x1920)</t>
+        </is>
+      </c>
+      <c r="I324" t="n">
+        <v>25</v>
+      </c>
+      <c r="J324" t="inlineStr">
+        <is>
+          <t>H265</t>
+        </is>
+      </c>
+      <c r="K324" t="n">
+        <v>1</v>
+      </c>
+      <c r="L324" t="n">
+        <v>30</v>
+      </c>
+      <c r="M324" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>Afsar Khan</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>REDX_VMS Portal</t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>Mumbai, Maharashtra</t>
+        </is>
+      </c>
+      <c r="D325" t="inlineStr">
+        <is>
+          <t>salman</t>
+        </is>
+      </c>
+      <c r="E325" t="n">
+        <v>4.17</v>
+      </c>
+      <c r="F325" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="G325" t="inlineStr">
+        <is>
+          <t>Honeywell</t>
+        </is>
+      </c>
+      <c r="H325" t="inlineStr">
+        <is>
+          <t>5MP (2560x1920)</t>
+        </is>
+      </c>
+      <c r="I325" t="n">
+        <v>25</v>
+      </c>
+      <c r="J325" t="inlineStr">
+        <is>
+          <t>H265</t>
+        </is>
+      </c>
+      <c r="K325" t="n">
+        <v>1</v>
+      </c>
+      <c r="L325" t="n">
+        <v>30</v>
+      </c>
+      <c r="M325" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>Afsar Khan</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>REDX_VMS Portal</t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>Mumbai, Maharashtra</t>
+        </is>
+      </c>
+      <c r="D326" t="inlineStr">
+        <is>
+          <t>salman</t>
+        </is>
+      </c>
+      <c r="E326" t="n">
+        <v>4.17</v>
+      </c>
+      <c r="F326" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="G326" t="inlineStr">
+        <is>
+          <t>Honeywell</t>
+        </is>
+      </c>
+      <c r="H326" t="inlineStr">
+        <is>
+          <t>5MP (2560x1920)</t>
+        </is>
+      </c>
+      <c r="I326" t="n">
+        <v>25</v>
+      </c>
+      <c r="J326" t="inlineStr">
+        <is>
+          <t>H265</t>
+        </is>
+      </c>
+      <c r="K326" t="n">
+        <v>1</v>
+      </c>
+      <c r="L326" t="n">
+        <v>30</v>
+      </c>
+      <c r="M326" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="D327" t="inlineStr">
+        <is>
+          <t>     </t>
+        </is>
+      </c>
+      <c r="E327" t="n">
+        <v>4.17</v>
+      </c>
+      <c r="F327" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="G327" t="inlineStr">
+        <is>
+          <t>Honeywell</t>
+        </is>
+      </c>
+      <c r="H327" t="inlineStr">
+        <is>
+          <t>5MP (2560x1920)</t>
+        </is>
+      </c>
+      <c r="I327" t="n">
+        <v>25</v>
+      </c>
+      <c r="J327" t="inlineStr">
+        <is>
+          <t>H265</t>
+        </is>
+      </c>
+      <c r="K327" t="n">
+        <v>1</v>
+      </c>
+      <c r="L327" t="n">
+        <v>30</v>
+      </c>
+      <c r="M327" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>  </t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>  </t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>  </t>
+        </is>
+      </c>
+      <c r="D328" t="inlineStr">
+        <is>
+          <t>  </t>
+        </is>
+      </c>
+      <c r="E328" t="n">
+        <v>4.17</v>
+      </c>
+      <c r="F328" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="G328" t="inlineStr">
+        <is>
+          <t>Honeywell</t>
+        </is>
+      </c>
+      <c r="H328" t="inlineStr">
+        <is>
+          <t>5MP (2560x1920)</t>
+        </is>
+      </c>
+      <c r="I328" t="n">
+        <v>25</v>
+      </c>
+      <c r="J328" t="inlineStr">
+        <is>
+          <t>H265</t>
+        </is>
+      </c>
+      <c r="K328" t="n">
+        <v>1</v>
+      </c>
+      <c r="L328" t="n">
+        <v>30</v>
+      </c>
+      <c r="M328" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>  </t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>  </t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>  </t>
+        </is>
+      </c>
+      <c r="D329" t="inlineStr">
+        <is>
+          <t>  </t>
+        </is>
+      </c>
+      <c r="E329" t="n">
+        <v>4.17</v>
+      </c>
+      <c r="F329" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="G329" t="inlineStr">
+        <is>
+          <t>Honeywell</t>
+        </is>
+      </c>
+      <c r="H329" t="inlineStr">
+        <is>
+          <t>5MP (2560x1920)</t>
+        </is>
+      </c>
+      <c r="I329" t="n">
+        <v>25</v>
+      </c>
+      <c r="J329" t="inlineStr">
+        <is>
+          <t>H265</t>
+        </is>
+      </c>
+      <c r="K329" t="n">
+        <v>1</v>
+      </c>
+      <c r="L329" t="n">
+        <v>30</v>
+      </c>
+      <c r="M329" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>  </t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>  </t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>  </t>
+        </is>
+      </c>
+      <c r="D330" t="inlineStr">
+        <is>
+          <t>  </t>
+        </is>
+      </c>
+      <c r="E330" t="n">
+        <v>4.17</v>
+      </c>
+      <c r="F330" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="G330" t="inlineStr">
+        <is>
+          <t>Honeywell</t>
+        </is>
+      </c>
+      <c r="H330" t="inlineStr">
+        <is>
+          <t>5MP (2560x1920)</t>
+        </is>
+      </c>
+      <c r="I330" t="n">
+        <v>25</v>
+      </c>
+      <c r="J330" t="inlineStr">
+        <is>
+          <t>H265</t>
+        </is>
+      </c>
+      <c r="K330" t="n">
+        <v>1</v>
+      </c>
+      <c r="L330" t="n">
+        <v>30</v>
+      </c>
+      <c r="M330" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="D331" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="E331" t="n">
+        <v>4.17</v>
+      </c>
+      <c r="F331" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="G331" t="inlineStr">
+        <is>
+          <t>Honeywell</t>
+        </is>
+      </c>
+      <c r="H331" t="inlineStr">
+        <is>
+          <t>5MP (2560x1920)</t>
+        </is>
+      </c>
+      <c r="I331" t="n">
+        <v>25</v>
+      </c>
+      <c r="J331" t="inlineStr">
+        <is>
+          <t>H265</t>
+        </is>
+      </c>
+      <c r="K331" t="n">
+        <v>1</v>
+      </c>
+      <c r="L331" t="n">
+        <v>30</v>
+      </c>
+      <c r="M331" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="D332" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="E332" t="n">
+        <v>4.17</v>
+      </c>
+      <c r="F332" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="G332" t="inlineStr">
+        <is>
+          <t>Honeywell</t>
+        </is>
+      </c>
+      <c r="H332" t="inlineStr">
+        <is>
+          <t>5MP (2560x1920)</t>
+        </is>
+      </c>
+      <c r="I332" t="n">
+        <v>25</v>
+      </c>
+      <c r="J332" t="inlineStr">
+        <is>
+          <t>H265</t>
+        </is>
+      </c>
+      <c r="K332" t="n">
+        <v>1</v>
+      </c>
+      <c r="L332" t="n">
+        <v>30</v>
+      </c>
+      <c r="M332" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="D333" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="E333" t="n">
+        <v>4.17</v>
+      </c>
+      <c r="F333" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="G333" t="inlineStr">
+        <is>
+          <t>Honeywell</t>
+        </is>
+      </c>
+      <c r="H333" t="inlineStr">
+        <is>
+          <t>5MP (2560x1920)</t>
+        </is>
+      </c>
+      <c r="I333" t="n">
+        <v>25</v>
+      </c>
+      <c r="J333" t="inlineStr">
+        <is>
+          <t>H265</t>
+        </is>
+      </c>
+      <c r="K333" t="n">
+        <v>1</v>
+      </c>
+      <c r="L333" t="n">
+        <v>30</v>
+      </c>
+      <c r="M333" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>  </t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>  </t>
+        </is>
+      </c>
+      <c r="D334" t="inlineStr">
+        <is>
+          <t>  </t>
+        </is>
+      </c>
+      <c r="E334" t="n">
+        <v>4.17</v>
+      </c>
+      <c r="F334" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="G334" t="inlineStr">
+        <is>
+          <t>Honeywell</t>
+        </is>
+      </c>
+      <c r="H334" t="inlineStr">
+        <is>
+          <t>5MP (2560x1920)</t>
+        </is>
+      </c>
+      <c r="I334" t="n">
+        <v>25</v>
+      </c>
+      <c r="J334" t="inlineStr">
+        <is>
+          <t>H265</t>
+        </is>
+      </c>
+      <c r="K334" t="n">
+        <v>1</v>
+      </c>
+      <c r="L334" t="n">
+        <v>30</v>
+      </c>
+      <c r="M334" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>  </t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>  </t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>  </t>
+        </is>
+      </c>
+      <c r="D335" t="inlineStr">
+        <is>
+          <t>  </t>
+        </is>
+      </c>
+      <c r="E335" t="n">
+        <v>4.17</v>
+      </c>
+      <c r="F335" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="G335" t="inlineStr">
+        <is>
+          <t>Honeywell</t>
+        </is>
+      </c>
+      <c r="H335" t="inlineStr">
+        <is>
+          <t>5MP (2560x1920)</t>
+        </is>
+      </c>
+      <c r="I335" t="n">
+        <v>25</v>
+      </c>
+      <c r="J335" t="inlineStr">
+        <is>
+          <t>H265</t>
+        </is>
+      </c>
+      <c r="K335" t="n">
+        <v>1</v>
+      </c>
+      <c r="L335" t="n">
+        <v>30</v>
+      </c>
+      <c r="M335" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>  </t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t>  </t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>  </t>
+        </is>
+      </c>
+      <c r="D336" t="inlineStr">
+        <is>
+          <t>  </t>
+        </is>
+      </c>
+      <c r="E336" t="n">
+        <v>4.17</v>
+      </c>
+      <c r="F336" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="G336" t="inlineStr">
+        <is>
+          <t>Honeywell</t>
+        </is>
+      </c>
+      <c r="H336" t="inlineStr">
+        <is>
+          <t>5MP (2560x1920)</t>
+        </is>
+      </c>
+      <c r="I336" t="n">
+        <v>25</v>
+      </c>
+      <c r="J336" t="inlineStr">
+        <is>
+          <t>H265</t>
+        </is>
+      </c>
+      <c r="K336" t="n">
+        <v>1</v>
+      </c>
+      <c r="L336" t="n">
+        <v>30</v>
+      </c>
+      <c r="M336" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>  </t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t>  </t>
+        </is>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>  </t>
+        </is>
+      </c>
+      <c r="D337" t="inlineStr">
+        <is>
+          <t>  </t>
+        </is>
+      </c>
+      <c r="E337" t="n">
+        <v>4.17</v>
+      </c>
+      <c r="F337" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="G337" t="inlineStr">
+        <is>
+          <t>Honeywell</t>
+        </is>
+      </c>
+      <c r="H337" t="inlineStr">
+        <is>
+          <t>5MP (2560x1920)</t>
+        </is>
+      </c>
+      <c r="I337" t="n">
+        <v>25</v>
+      </c>
+      <c r="J337" t="inlineStr">
+        <is>
+          <t>H265</t>
+        </is>
+      </c>
+      <c r="K337" t="n">
+        <v>1</v>
+      </c>
+      <c r="L337" t="n">
+        <v>30</v>
+      </c>
+      <c r="M337" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>  </t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>  </t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>  </t>
+        </is>
+      </c>
+      <c r="D338" t="inlineStr">
+        <is>
+          <t>  </t>
+        </is>
+      </c>
+      <c r="E338" t="n">
+        <v>4.17</v>
+      </c>
+      <c r="F338" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="G338" t="inlineStr">
+        <is>
+          <t>Honeywell</t>
+        </is>
+      </c>
+      <c r="H338" t="inlineStr">
+        <is>
+          <t>5MP (2560x1920)</t>
+        </is>
+      </c>
+      <c r="I338" t="n">
+        <v>25</v>
+      </c>
+      <c r="J338" t="inlineStr">
+        <is>
+          <t>H265</t>
+        </is>
+      </c>
+      <c r="K338" t="n">
+        <v>1</v>
+      </c>
+      <c r="L338" t="n">
+        <v>30</v>
+      </c>
+      <c r="M338" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>Afsar Khan</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>REDX_VMS</t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>Mumbai</t>
+        </is>
+      </c>
+      <c r="D339" t="inlineStr">
+        <is>
+          <t>Mr.Gagan</t>
+        </is>
+      </c>
+      <c r="E339" t="n">
+        <v>4.17</v>
+      </c>
+      <c r="F339" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="G339" t="inlineStr">
+        <is>
+          <t>Honeywell</t>
+        </is>
+      </c>
+      <c r="H339" t="inlineStr">
+        <is>
+          <t>5MP (2560x1920)</t>
+        </is>
+      </c>
+      <c r="I339" t="n">
+        <v>25</v>
+      </c>
+      <c r="J339" t="inlineStr">
+        <is>
+          <t>H265</t>
+        </is>
+      </c>
+      <c r="K339" t="n">
+        <v>1</v>
+      </c>
+      <c r="L339" t="n">
+        <v>30</v>
+      </c>
+      <c r="M339" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>Afsar</t>
+        </is>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>REDX_Portal</t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>Mumbai, Maharashtra, India, 400059</t>
+        </is>
+      </c>
+      <c r="D340" t="inlineStr">
+        <is>
+          <t>Mr.Nitin</t>
+        </is>
+      </c>
+      <c r="E340" t="n">
+        <v>4.17</v>
+      </c>
+      <c r="F340" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="G340" t="inlineStr">
+        <is>
+          <t>Honeywell</t>
+        </is>
+      </c>
+      <c r="H340" t="inlineStr">
+        <is>
+          <t>5MP (2560x1920)</t>
+        </is>
+      </c>
+      <c r="I340" t="n">
+        <v>25</v>
+      </c>
+      <c r="J340" t="inlineStr">
+        <is>
+          <t>H265</t>
+        </is>
+      </c>
+      <c r="K340" t="n">
+        <v>1</v>
+      </c>
+      <c r="L340" t="n">
+        <v>30</v>
+      </c>
+      <c r="M340" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>  </t>
+        </is>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t>  </t>
+        </is>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>  </t>
+        </is>
+      </c>
+      <c r="D341" t="inlineStr">
+        <is>
+          <t>  </t>
+        </is>
+      </c>
+      <c r="E341" t="n">
+        <v>4.17</v>
+      </c>
+      <c r="F341" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="G341" t="inlineStr">
+        <is>
+          <t>Honeywell</t>
+        </is>
+      </c>
+      <c r="H341" t="inlineStr">
+        <is>
+          <t>5MP (2560x1920)</t>
+        </is>
+      </c>
+      <c r="I341" t="n">
+        <v>25</v>
+      </c>
+      <c r="J341" t="inlineStr">
+        <is>
+          <t>H265</t>
+        </is>
+      </c>
+      <c r="K341" t="n">
+        <v>1</v>
+      </c>
+      <c r="L341" t="n">
+        <v>30</v>
+      </c>
+      <c r="M341" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Solve bug in data history and Authentication using JWT
</commit_message>
<xml_diff>
--- a/backend/exports/all_requirements.xlsx
+++ b/backend/exports/all_requirements.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M341"/>
+  <dimension ref="A1:M347"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -19060,6 +19060,336 @@
         <v>1</v>
       </c>
     </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>Afsar Khan</t>
+        </is>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t>REDX_VMS Portal</t>
+        </is>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>Mumbai Maharashtra India</t>
+        </is>
+      </c>
+      <c r="D342" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="E342" t="n">
+        <v>4.17</v>
+      </c>
+      <c r="F342" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="G342" t="inlineStr">
+        <is>
+          <t>Honeywell</t>
+        </is>
+      </c>
+      <c r="H342" t="inlineStr">
+        <is>
+          <t>5MP (2560x1920)</t>
+        </is>
+      </c>
+      <c r="I342" t="n">
+        <v>25</v>
+      </c>
+      <c r="J342" t="inlineStr">
+        <is>
+          <t>H265</t>
+        </is>
+      </c>
+      <c r="K342" t="n">
+        <v>1</v>
+      </c>
+      <c r="L342" t="n">
+        <v>30</v>
+      </c>
+      <c r="M342" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>AK</t>
+        </is>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>REDX_VMS Portal</t>
+        </is>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>Kothrud, Pune, Maharashtra, India</t>
+        </is>
+      </c>
+      <c r="D343" t="inlineStr">
+        <is>
+          <t>Dallas</t>
+        </is>
+      </c>
+      <c r="E343" t="n">
+        <v>4.17</v>
+      </c>
+      <c r="F343" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="G343" t="inlineStr">
+        <is>
+          <t>Honeywell</t>
+        </is>
+      </c>
+      <c r="H343" t="inlineStr">
+        <is>
+          <t>5MP (2560x1920)</t>
+        </is>
+      </c>
+      <c r="I343" t="n">
+        <v>25</v>
+      </c>
+      <c r="J343" t="inlineStr">
+        <is>
+          <t>H265</t>
+        </is>
+      </c>
+      <c r="K343" t="n">
+        <v>1</v>
+      </c>
+      <c r="L343" t="n">
+        <v>30</v>
+      </c>
+      <c r="M343" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>AK</t>
+        </is>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>REDX_VMS Portal</t>
+        </is>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>Kothrud, Pune, Maharashtra, India</t>
+        </is>
+      </c>
+      <c r="D344" t="inlineStr">
+        <is>
+          <t>Dallas</t>
+        </is>
+      </c>
+      <c r="E344" t="n">
+        <v>4.17</v>
+      </c>
+      <c r="F344" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="G344" t="inlineStr">
+        <is>
+          <t>Honeywell</t>
+        </is>
+      </c>
+      <c r="H344" t="inlineStr">
+        <is>
+          <t>5MP (2560x1920)</t>
+        </is>
+      </c>
+      <c r="I344" t="n">
+        <v>25</v>
+      </c>
+      <c r="J344" t="inlineStr">
+        <is>
+          <t>H265</t>
+        </is>
+      </c>
+      <c r="K344" t="n">
+        <v>1</v>
+      </c>
+      <c r="L344" t="n">
+        <v>30</v>
+      </c>
+      <c r="M344" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>AK</t>
+        </is>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>REDX_VMS Portal</t>
+        </is>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>Kothrud, Pune, Maharashtra, India</t>
+        </is>
+      </c>
+      <c r="D345" t="inlineStr">
+        <is>
+          <t>Dallas</t>
+        </is>
+      </c>
+      <c r="E345" t="n">
+        <v>4.17</v>
+      </c>
+      <c r="F345" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="G345" t="inlineStr">
+        <is>
+          <t>Honeywell</t>
+        </is>
+      </c>
+      <c r="H345" t="inlineStr">
+        <is>
+          <t>5MP (2560x1920)</t>
+        </is>
+      </c>
+      <c r="I345" t="n">
+        <v>25</v>
+      </c>
+      <c r="J345" t="inlineStr">
+        <is>
+          <t>H265</t>
+        </is>
+      </c>
+      <c r="K345" t="n">
+        <v>1</v>
+      </c>
+      <c r="L345" t="n">
+        <v>30</v>
+      </c>
+      <c r="M345" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>AK</t>
+        </is>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t>REDX_VMS Portal</t>
+        </is>
+      </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>Kothrud, Pune, Maharashtra, India</t>
+        </is>
+      </c>
+      <c r="D346" t="inlineStr">
+        <is>
+          <t>Dallas</t>
+        </is>
+      </c>
+      <c r="E346" t="n">
+        <v>4.17</v>
+      </c>
+      <c r="F346" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="G346" t="inlineStr">
+        <is>
+          <t>Honeywell</t>
+        </is>
+      </c>
+      <c r="H346" t="inlineStr">
+        <is>
+          <t>5MP (2560x1920)</t>
+        </is>
+      </c>
+      <c r="I346" t="n">
+        <v>25</v>
+      </c>
+      <c r="J346" t="inlineStr">
+        <is>
+          <t>H265</t>
+        </is>
+      </c>
+      <c r="K346" t="n">
+        <v>1</v>
+      </c>
+      <c r="L346" t="n">
+        <v>30</v>
+      </c>
+      <c r="M346" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>  </t>
+        </is>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t>  </t>
+        </is>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>  </t>
+        </is>
+      </c>
+      <c r="D347" t="inlineStr">
+        <is>
+          <t>  </t>
+        </is>
+      </c>
+      <c r="E347" t="n">
+        <v>4.17</v>
+      </c>
+      <c r="F347" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="G347" t="inlineStr">
+        <is>
+          <t>Honeywell</t>
+        </is>
+      </c>
+      <c r="H347" t="inlineStr">
+        <is>
+          <t>5MP (2560x1920)</t>
+        </is>
+      </c>
+      <c r="I347" t="n">
+        <v>25</v>
+      </c>
+      <c r="J347" t="inlineStr">
+        <is>
+          <t>H265</t>
+        </is>
+      </c>
+      <c r="K347" t="n">
+        <v>1</v>
+      </c>
+      <c r="L347" t="n">
+        <v>30</v>
+      </c>
+      <c r="M347" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>